<commit_message>
update factory for diagonal
</commit_message>
<xml_diff>
--- a/CW1/results/results.xlsx
+++ b/CW1/results/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10203"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA5C923-9D79-4D15-855F-8CA3E6D69168}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0E15CF-4C10-4643-92C1-AB1CBD7061E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9936" yWindow="888" windowWidth="12432" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="21">
   <si>
     <t>lines map</t>
   </si>
@@ -94,7 +94,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,7 +149,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -487,20 +487,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="3" width="10.44140625" customWidth="1"/>
+    <col min="2" max="3" width="10.5" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -529,12 +529,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -566,7 +566,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -598,7 +598,7 @@
         <v>1531.87</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -630,7 +630,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -662,7 +662,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -694,12 +694,12 @@
         <v>38205</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -731,7 +731,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -763,7 +763,7 @@
         <v>2041.02</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -795,7 +795,7 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -827,7 +827,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -859,12 +859,12 @@
         <v>38205</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -896,7 +896,7 @@
         <v>1523</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -928,7 +928,7 @@
         <v>1995.76</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -960,7 +960,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -992,7 +992,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1024,12 +1024,12 @@
         <v>10620</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>359.09</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>12</v>
       </c>
@@ -1208,6 +1208,9 @@
       <c r="G29" t="s">
         <v>17</v>
       </c>
+      <c r="H29" t="s">
+        <v>20</v>
+      </c>
       <c r="I29" t="s">
         <v>18</v>
       </c>
@@ -1215,12 +1218,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1252,7 +1255,7 @@
         <v>4255</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>423.42</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1348,7 +1351,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1380,12 +1383,12 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1407,6 +1410,9 @@
       <c r="G38">
         <v>3921</v>
       </c>
+      <c r="H38">
+        <v>3947</v>
+      </c>
       <c r="I38">
         <v>4510</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>5316</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1436,6 +1442,9 @@
       <c r="G39">
         <v>131.63</v>
       </c>
+      <c r="H39">
+        <v>113.9</v>
+      </c>
       <c r="I39">
         <v>133.11000000000001</v>
       </c>
@@ -1443,7 +1452,7 @@
         <v>286.83999999999997</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1465,6 +1474,9 @@
       <c r="G40">
         <v>93</v>
       </c>
+      <c r="H40">
+        <v>93</v>
+      </c>
       <c r="I40">
         <v>91</v>
       </c>
@@ -1472,7 +1484,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1494,6 +1506,9 @@
       <c r="G41">
         <v>108</v>
       </c>
+      <c r="H41">
+        <v>106</v>
+      </c>
       <c r="I41">
         <v>110</v>
       </c>
@@ -1501,7 +1516,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1523,6 +1538,9 @@
       <c r="G42">
         <v>855</v>
       </c>
+      <c r="H42">
+        <v>675</v>
+      </c>
       <c r="I42">
         <v>810</v>
       </c>
@@ -1530,7 +1548,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -1544,7 +1562,7 @@
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1566,7 +1584,9 @@
       <c r="G45" s="1">
         <v>3920</v>
       </c>
-      <c r="H45" s="1"/>
+      <c r="H45" s="1">
+        <v>3946</v>
+      </c>
       <c r="I45" s="1">
         <v>4510</v>
       </c>
@@ -1574,7 +1594,7 @@
         <v>5316</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
@@ -1596,7 +1616,9 @@
       <c r="G46" s="1">
         <v>136.4</v>
       </c>
-      <c r="H46" s="1"/>
+      <c r="H46" s="1">
+        <v>117.6</v>
+      </c>
       <c r="I46" s="1">
         <v>137.47999999999999</v>
       </c>
@@ -1604,7 +1626,7 @@
         <v>292.02</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
@@ -1626,7 +1648,9 @@
       <c r="G47" s="1">
         <v>93</v>
       </c>
-      <c r="H47" s="1"/>
+      <c r="H47" s="1">
+        <v>93</v>
+      </c>
       <c r="I47" s="1">
         <v>91</v>
       </c>
@@ -1634,7 +1658,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>6</v>
       </c>
@@ -1656,7 +1680,9 @@
       <c r="G48" s="1">
         <v>110</v>
       </c>
-      <c r="H48" s="1"/>
+      <c r="H48" s="1">
+        <v>110</v>
+      </c>
       <c r="I48" s="1">
         <v>110</v>
       </c>
@@ -1664,7 +1690,7 @@
         <v>1537</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -1686,7 +1712,9 @@
       <c r="G49" s="1">
         <v>855</v>
       </c>
-      <c r="H49" s="1"/>
+      <c r="H49" s="1">
+        <v>540</v>
+      </c>
       <c r="I49" s="1">
         <v>810</v>
       </c>
@@ -1694,7 +1722,7 @@
         <v>2385</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>12</v>
       </c>
@@ -1712,6 +1740,9 @@
       </c>
       <c r="G50" t="s">
         <v>17</v>
+      </c>
+      <c r="H50" t="s">
+        <v>20</v>
       </c>
       <c r="I50" t="s">
         <v>18</v>
@@ -1733,7 +1764,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1747,7 +1778,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update AD+AE in factory_terrain
</commit_message>
<xml_diff>
--- a/CW1/results/results.xlsx
+++ b/CW1/results/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10203"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FA7FD8-AED7-49A1-A9E5-87C7FF63D699}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9EA6A8-CDD3-954E-87CF-139981C2AE6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5412" yWindow="2220" windowWidth="12768" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-500" yWindow="460" windowWidth="24120" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
   <si>
     <t>lines map</t>
   </si>
@@ -124,13 +124,28 @@
   </si>
   <si>
     <t>AE 10</t>
+  </si>
+  <si>
+    <t>factory</t>
+  </si>
+  <si>
+    <t>factory_terrain</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AD 0.5</t>
+  </si>
+  <si>
+    <t>AD 10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,7 +206,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -204,9 +219,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -222,7 +238,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -542,24 +558,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="4" max="5" width="10.44140625" customWidth="1"/>
+    <col min="4" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -597,12 +613,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -643,7 +659,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -684,7 +700,7 @@
         <v>93.86</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -725,7 +741,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -766,7 +782,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -807,12 +823,12 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -853,7 +869,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -894,7 +910,7 @@
         <v>108.21</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -935,7 +951,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -976,7 +992,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1017,12 +1033,12 @@
         <v>945</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1063,7 +1079,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1104,7 +1120,7 @@
         <v>110.01</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1145,7 +1161,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -1186,7 +1202,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1227,12 +1243,12 @@
         <v>720</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1289,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -1314,7 +1330,7 @@
         <v>62.66</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1355,7 +1371,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1396,7 +1412,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1437,7 +1453,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>18</v>
       </c>
@@ -1475,12 +1491,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -1521,7 +1537,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -1562,7 +1578,7 @@
         <v>66.52</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1603,7 +1619,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>6</v>
       </c>
@@ -1644,7 +1660,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1685,12 +1701,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1731,7 +1747,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>1</v>
       </c>
@@ -1772,7 +1788,7 @@
         <v>115.1</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -1813,7 +1829,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1854,7 +1870,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -1895,7 +1911,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -1910,7 +1926,7 @@
       <c r="J44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>3</v>
       </c>
@@ -1951,7 +1967,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
@@ -1992,7 +2008,7 @@
         <v>116.2</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>2</v>
       </c>
@@ -2033,7 +2049,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>6</v>
       </c>
@@ -2074,7 +2090,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>7</v>
       </c>
@@ -2115,7 +2131,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>18</v>
       </c>
@@ -2153,7 +2169,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>33</v>
+      </c>
+      <c r="H55" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>23</v>
       </c>
@@ -2169,8 +2193,23 @@
       <c r="E56" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="57" spans="1:15">
+      <c r="H56" t="s">
+        <v>23</v>
+      </c>
+      <c r="I56" t="s">
+        <v>27</v>
+      </c>
+      <c r="J56" t="s">
+        <v>28</v>
+      </c>
+      <c r="K56" t="s">
+        <v>29</v>
+      </c>
+      <c r="L56" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -2186,8 +2225,23 @@
       <c r="E57">
         <v>20.51</v>
       </c>
-    </row>
-    <row r="58" spans="1:15">
+      <c r="H57" t="s">
+        <v>24</v>
+      </c>
+      <c r="I57" s="4">
+        <v>24.12</v>
+      </c>
+      <c r="J57" s="4">
+        <v>18.329999999999998</v>
+      </c>
+      <c r="K57" s="4">
+        <v>14.78</v>
+      </c>
+      <c r="L57" s="4">
+        <v>20.61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>25</v>
       </c>
@@ -2203,8 +2257,23 @@
       <c r="E58">
         <v>992.5</v>
       </c>
-    </row>
-    <row r="59" spans="1:15">
+      <c r="H58" t="s">
+        <v>25</v>
+      </c>
+      <c r="I58" s="4">
+        <v>1302.73</v>
+      </c>
+      <c r="J58" s="4">
+        <v>1247.4100000000001</v>
+      </c>
+      <c r="K58" s="4">
+        <v>455.7</v>
+      </c>
+      <c r="L58" s="4">
+        <v>1851.29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>26</v>
       </c>
@@ -2220,13 +2289,31 @@
       <c r="E59">
         <v>150.31</v>
       </c>
-    </row>
-    <row r="61" spans="1:15">
+      <c r="H59" t="s">
+        <v>26</v>
+      </c>
+      <c r="I59" s="4">
+        <v>180.68</v>
+      </c>
+      <c r="J59" s="4">
+        <v>135.26</v>
+      </c>
+      <c r="K59" s="4">
+        <v>108.23</v>
+      </c>
+      <c r="L59" s="4">
+        <v>158.47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="62" spans="1:15">
+      <c r="H61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -2242,8 +2329,23 @@
       <c r="E62">
         <v>20.47</v>
       </c>
-    </row>
-    <row r="63" spans="1:15">
+      <c r="H62" t="s">
+        <v>24</v>
+      </c>
+      <c r="I62" s="4">
+        <v>23.56</v>
+      </c>
+      <c r="J62" s="4">
+        <v>18.170000000000002</v>
+      </c>
+      <c r="K62" s="4">
+        <v>14.73</v>
+      </c>
+      <c r="L62" s="4">
+        <v>20.48</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -2259,8 +2361,23 @@
       <c r="E63">
         <v>1265.2</v>
       </c>
-    </row>
-    <row r="64" spans="1:15">
+      <c r="H63" t="s">
+        <v>25</v>
+      </c>
+      <c r="I63" s="4">
+        <v>1146.8399999999999</v>
+      </c>
+      <c r="J63" s="4">
+        <v>916.05</v>
+      </c>
+      <c r="K63" s="4">
+        <v>874.63</v>
+      </c>
+      <c r="L63" s="4">
+        <v>1281.3499999999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -2276,13 +2393,31 @@
       <c r="E64">
         <v>152.13999999999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="H64" t="s">
+        <v>26</v>
+      </c>
+      <c r="I64" s="4">
+        <v>175.98</v>
+      </c>
+      <c r="J64" s="4">
+        <v>130.74</v>
+      </c>
+      <c r="K64" s="4">
+        <v>115.17</v>
+      </c>
+      <c r="L64" s="4">
+        <v>151.43</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="H67" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>24</v>
       </c>
@@ -2298,8 +2433,23 @@
       <c r="E68">
         <v>20.52</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="H68" t="s">
+        <v>24</v>
+      </c>
+      <c r="I68" s="4">
+        <v>24.84</v>
+      </c>
+      <c r="J68" s="4">
+        <v>22.97</v>
+      </c>
+      <c r="K68" s="4">
+        <v>14.95</v>
+      </c>
+      <c r="L68" s="4">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>25</v>
       </c>
@@ -2315,8 +2465,23 @@
       <c r="E69">
         <v>962.3</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="H69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I69" s="4">
+        <v>871.23</v>
+      </c>
+      <c r="J69" s="4">
+        <v>2636.26</v>
+      </c>
+      <c r="K69" s="4">
+        <v>627.74</v>
+      </c>
+      <c r="L69" s="4">
+        <v>2868.05</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -2331,6 +2496,212 @@
       </c>
       <c r="E70">
         <v>146.16999999999999</v>
+      </c>
+      <c r="H70" t="s">
+        <v>26</v>
+      </c>
+      <c r="I70" s="4">
+        <v>176.95</v>
+      </c>
+      <c r="J70" s="4">
+        <v>176.64</v>
+      </c>
+      <c r="K70" s="4">
+        <v>111.96</v>
+      </c>
+      <c r="L70" s="4">
+        <v>179.47</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>35</v>
+      </c>
+      <c r="I74" t="s">
+        <v>27</v>
+      </c>
+      <c r="J74" t="s">
+        <v>28</v>
+      </c>
+      <c r="K74" t="s">
+        <v>29</v>
+      </c>
+      <c r="L74" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>24</v>
+      </c>
+      <c r="I75" s="4">
+        <v>23.4</v>
+      </c>
+      <c r="J75" s="4">
+        <v>18.18</v>
+      </c>
+      <c r="K75" s="4">
+        <v>14.21</v>
+      </c>
+      <c r="L75" s="4">
+        <v>20.49</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H76" t="s">
+        <v>25</v>
+      </c>
+      <c r="I76" s="4">
+        <v>811.91</v>
+      </c>
+      <c r="J76" s="4">
+        <v>932.45</v>
+      </c>
+      <c r="K76" s="4">
+        <v>2126.2600000000002</v>
+      </c>
+      <c r="L76" s="4">
+        <v>1131.79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>26</v>
+      </c>
+      <c r="I77" s="4">
+        <v>170.24</v>
+      </c>
+      <c r="J77" s="4">
+        <v>130.53</v>
+      </c>
+      <c r="K77" s="4">
+        <v>155.55000000000001</v>
+      </c>
+      <c r="L77" s="4">
+        <v>152.51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>24</v>
+      </c>
+      <c r="I80" s="4">
+        <v>23.36</v>
+      </c>
+      <c r="J80" s="4">
+        <v>18.18</v>
+      </c>
+      <c r="K80" s="4">
+        <v>14.69</v>
+      </c>
+      <c r="L80" s="4">
+        <v>20.48</v>
+      </c>
+    </row>
+    <row r="81" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H81" t="s">
+        <v>25</v>
+      </c>
+      <c r="I81" s="4">
+        <v>1081.4000000000001</v>
+      </c>
+      <c r="J81" s="4">
+        <v>920.26</v>
+      </c>
+      <c r="K81" s="4">
+        <v>1140.42</v>
+      </c>
+      <c r="L81" s="4">
+        <v>1300.8399999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>26</v>
+      </c>
+      <c r="I82" s="4">
+        <v>173.5</v>
+      </c>
+      <c r="J82" s="4">
+        <v>129.93</v>
+      </c>
+      <c r="K82" s="4">
+        <v>113.74</v>
+      </c>
+      <c r="L82" s="4">
+        <v>153.76</v>
+      </c>
+    </row>
+    <row r="85" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="86" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>24</v>
+      </c>
+      <c r="I86" s="4">
+        <v>24.01</v>
+      </c>
+      <c r="J86" s="4">
+        <v>18.809999999999999</v>
+      </c>
+      <c r="K86" s="4">
+        <v>14.95</v>
+      </c>
+      <c r="L86" s="4">
+        <v>24.82</v>
+      </c>
+    </row>
+    <row r="87" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>25</v>
+      </c>
+      <c r="I87" s="4">
+        <v>542.54</v>
+      </c>
+      <c r="J87" s="4">
+        <v>951.41</v>
+      </c>
+      <c r="K87" s="4">
+        <v>627.74</v>
+      </c>
+      <c r="L87" s="4">
+        <v>1249.6600000000001</v>
+      </c>
+    </row>
+    <row r="88" spans="8:12" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>26</v>
+      </c>
+      <c r="I88" s="4">
+        <v>176.78</v>
+      </c>
+      <c r="J88" s="4">
+        <v>136.79</v>
+      </c>
+      <c r="K88" s="4">
+        <v>111.96</v>
+      </c>
+      <c r="L88" s="4">
+        <v>187.91</v>
       </c>
     </row>
   </sheetData>
@@ -2346,7 +2717,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2360,7 +2731,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
D/A/T charts for factory map
</commit_message>
<xml_diff>
--- a/CW1/results/results.xlsx
+++ b/CW1/results/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C7BBD6-2E32-0A45-AE64-3843A091AA6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC1F2235-F501-44C8-868E-8E76BE2F1E48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="58">
   <si>
     <t>lines map</t>
   </si>
@@ -175,6 +177,46 @@
   <si>
     <t>sum</t>
   </si>
+  <si>
+    <t>total distance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Algorithm</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total Angle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>total time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A* Euclidean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A* Euclidean 0.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A* Euclidean 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A* Diagonal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A* Diagonal 0.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A* Diagonal 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -184,7 +226,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -192,13 +234,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -206,7 +248,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -214,7 +256,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -278,7 +320,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -352,7 +394,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -694,7 +736,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1142320776"/>
@@ -754,7 +796,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1142325696"/>
@@ -796,7 +838,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -826,7 +868,993 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Total Distance on Factory Map</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total distance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$E$13:$E$18</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>A* Euclidean</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A* Euclidean 0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>A* Euclidean 10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A* Diagonal</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>A* Diagonal 0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>A* Diagonal 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$13:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>76.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.959999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>83.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.320000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>82.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4FDE-4CD6-8C45-C7A638379629}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="801989376"/>
+        <c:axId val="801993968"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="801989376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="801993968"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="801993968"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="801989376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" altLang="zh-CN"/>
+              <a:t>Total Angle </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>on Factory Map</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$J$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total Angle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$I$13:$I$18</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>A* Euclidean</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A* Euclidean 0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>A* Euclidean 10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A* Diagonal</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>A* Diagonal 0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>A* Diagonal 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$13:$J$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4732.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4215.7199999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4301.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4508.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6584.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3067.3199999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC70-48D9-AE6B-926A05611346}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="807353728"/>
+        <c:axId val="807357336"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="807353728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="807357336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="807357336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="807353728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" altLang="zh-CN"/>
+              <a:t>Total Time </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>on Factory Map</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" altLang="zh-CN"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$N$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>total time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$M$13:$M$18</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>A* Euclidean</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A* Euclidean 0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>A* Euclidean 10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>A* Diagonal</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>A* Diagonal 0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>A* Diagonal 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$N$13:$N$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>563.32000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>557.67999999999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>604.68999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>566.57000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>569.34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>602.41999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A3E-4508-83CD-926A96AAD2BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="802013648"/>
+        <c:axId val="802016928"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="802013648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="802016928"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="802016928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="802013648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -877,7 +1905,1636 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1413,6 +4070,120 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>918483</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>11338</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>376465</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>33109</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A77BDF6-25E5-42DD-90A5-511CBDAB1929}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>884464</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>113392</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>342446</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>135164</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4083E13C-5FE3-4631-95F0-11ECD7BAE8FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>430892</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>240392</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>101146</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEA3AB57-6D75-4C20-8001-41D7C81DC6AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1744,23 +4515,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" topLeftCell="D49" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W88" sqref="W88"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="4" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="25.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.125" customWidth="1"/>
+    <col min="13" max="13" width="13.625" customWidth="1"/>
     <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -1798,12 +4569,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1844,7 +4615,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1885,7 +4656,7 @@
         <v>93.86</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1926,7 +4697,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1967,7 +4738,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2008,12 +4779,12 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2054,7 +4825,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2095,7 +4866,7 @@
         <v>108.21</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2136,7 +4907,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2177,7 +4948,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -2218,12 +4989,12 @@
         <v>945</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -2264,7 +5035,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -2305,7 +5076,7 @@
         <v>110.01</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2346,7 +5117,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -2387,7 +5158,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -2428,12 +5199,12 @@
         <v>720</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -2474,7 +5245,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -2515,7 +5286,7 @@
         <v>62.66</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -2556,7 +5327,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -2597,7 +5368,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -2638,7 +5409,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>18</v>
       </c>
@@ -2676,12 +5447,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -2722,7 +5493,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -2763,7 +5534,7 @@
         <v>66.52</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -2804,7 +5575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -2845,7 +5616,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -2886,12 +5657,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -2932,7 +5703,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -2973,7 +5744,7 @@
         <v>115.1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -3014,7 +5785,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -3055,7 +5826,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -3096,7 +5867,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -3111,7 +5882,7 @@
       <c r="J47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>3</v>
       </c>
@@ -3152,7 +5923,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>1</v>
       </c>
@@ -3193,7 +5964,7 @@
         <v>116.2</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>2</v>
       </c>
@@ -3234,7 +6005,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>6</v>
       </c>
@@ -3275,7 +6046,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -3316,7 +6087,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3324,7 +6095,7 @@
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3332,7 +6103,7 @@
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B55" t="s">
         <v>18</v>
       </c>
@@ -3370,12 +6141,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E57" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>33</v>
       </c>
@@ -3383,7 +6154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -3418,7 +6189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -3454,7 +6225,7 @@
         <v>20.61</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -3490,7 +6261,7 @@
         <v>1851.29</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -3526,7 +6297,7 @@
         <v>158.47</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A66" t="s">
         <v>31</v>
       </c>
@@ -3534,7 +6305,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A67" t="s">
         <v>24</v>
       </c>
@@ -3570,7 +6341,7 @@
         <v>20.48</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>25</v>
       </c>
@@ -3606,7 +6377,7 @@
         <v>1281.3499999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -3642,7 +6413,7 @@
         <v>151.43</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
         <v>32</v>
       </c>
@@ -3650,7 +6421,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
         <v>24</v>
       </c>
@@ -3686,7 +6457,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>25</v>
       </c>
@@ -3722,7 +6493,7 @@
         <v>2868.05</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>26</v>
       </c>
@@ -3758,7 +6529,7 @@
         <v>179.47</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>35</v>
       </c>
@@ -3767,7 +6538,7 @@
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -3791,7 +6562,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A79" t="s">
         <v>25</v>
       </c>
@@ -3827,7 +6598,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -3863,7 +6634,7 @@
         <v>20.49</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.15">
       <c r="H81" t="s">
         <v>25</v>
       </c>
@@ -3880,7 +6651,7 @@
         <v>1131.79</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>36</v>
       </c>
@@ -3900,7 +6671,7 @@
         <v>152.51</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -3921,7 +6692,7 @@
         <v>76.2</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>25</v>
       </c>
@@ -3945,7 +6716,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -3981,7 +6752,7 @@
         <v>20.48</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="H86" t="s">
         <v>25</v>
       </c>
@@ -3998,7 +6769,7 @@
         <v>1300.8399999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" t="s">
         <v>37</v>
       </c>
@@ -4018,7 +6789,7 @@
         <v>153.76</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A88" t="s">
         <v>24</v>
       </c>
@@ -4039,7 +6810,7 @@
         <v>82.43</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>25</v>
       </c>
@@ -4060,7 +6831,7 @@
         <v>3067.3199999999997</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>26</v>
       </c>
@@ -4084,7 +6855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
       <c r="H91" t="s">
         <v>24</v>
       </c>
@@ -4101,7 +6872,7 @@
         <v>24.82</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
       <c r="H92" t="s">
         <v>25</v>
       </c>
@@ -4118,7 +6889,7 @@
         <v>1249.6600000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
       <c r="H93" t="s">
         <v>26</v>
       </c>
@@ -4135,7 +6906,7 @@
         <v>187.91</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B98" t="s">
         <v>12</v>
       </c>
@@ -4158,7 +6929,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
       <c r="C99">
         <v>8.5</v>
       </c>
@@ -4181,7 +6952,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B100">
         <v>0</v>
       </c>
@@ -4225,7 +6996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B101">
         <v>0</v>
       </c>
@@ -4272,7 +7043,7 @@
         <v>4.7000000000000011</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B102">
         <v>0</v>
       </c>
@@ -4319,7 +7090,7 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B103">
         <v>0</v>
       </c>
@@ -4366,7 +7137,7 @@
         <v>0.73428571428571432</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B104">
         <v>0</v>
       </c>
@@ -4389,7 +7160,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B105" s="1">
         <v>0</v>
       </c>
@@ -4412,7 +7183,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A106" s="3" t="s">
         <v>39</v>
       </c>
@@ -4448,7 +7219,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
       <c r="L107" t="s">
         <v>12</v>
       </c>
@@ -4471,7 +7242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
       <c r="K108" t="s">
         <v>44</v>
       </c>
@@ -4485,7 +7256,7 @@
         <v>0.99</v>
       </c>
       <c r="O108" s="5">
-        <f t="shared" ref="L108:R108" si="1">O101/$M101</f>
+        <f t="shared" ref="O108:R108" si="1">O101/$M101</f>
         <v>0.21236133122028528</v>
       </c>
       <c r="P108" s="5">
@@ -4501,7 +7272,7 @@
         <v>0.52139461172741697</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B109">
         <v>0.14000000000000001</v>
       </c>
@@ -4530,7 +7301,7 @@
         <v>0.99</v>
       </c>
       <c r="M109" s="5">
-        <f t="shared" ref="L109:R110" si="2">M102/$L102</f>
+        <f t="shared" ref="M109:R110" si="2">M102/$L102</f>
         <v>2.6315789473684209E-2</v>
       </c>
       <c r="N109" s="5">
@@ -4554,7 +7325,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B110">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -4605,7 +7376,7 @@
         <v>0.65477707006369434</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B111">
         <v>0</v>
       </c>
@@ -4628,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B112">
         <v>0.01</v>
       </c>
@@ -4651,7 +7422,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B113">
         <v>0.27</v>
       </c>
@@ -4674,7 +7445,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B114" s="3">
         <v>0.27</v>
       </c>
@@ -4697,7 +7468,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
         <v>40</v>
       </c>
@@ -4729,7 +7500,7 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B117">
         <v>1.1000000000000001</v>
       </c>
@@ -4752,7 +7523,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B118">
         <v>2.34</v>
       </c>
@@ -4775,7 +7546,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B119">
         <v>0.86</v>
       </c>
@@ -4798,7 +7569,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B120">
         <v>0.04</v>
       </c>
@@ -4821,7 +7592,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B121">
         <v>0.05</v>
       </c>
@@ -4844,7 +7615,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B122" s="3">
         <v>1.63</v>
       </c>
@@ -4867,7 +7638,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B123">
         <v>1.83</v>
       </c>
@@ -4890,7 +7661,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A124" t="s">
         <v>41</v>
       </c>
@@ -4933,12 +7704,214 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="E11:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12:N18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="5" max="5" width="19.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13">
+        <v>76.69</v>
+      </c>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13">
+        <v>4732.5</v>
+      </c>
+      <c r="M13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13">
+        <v>563.32000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14">
+        <v>75.959999999999994</v>
+      </c>
+      <c r="I14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14">
+        <v>4215.7199999999993</v>
+      </c>
+      <c r="M14" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14">
+        <v>557.67999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15">
+        <v>83.5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J15">
+        <v>4301.2</v>
+      </c>
+      <c r="M15" t="s">
+        <v>54</v>
+      </c>
+      <c r="N15">
+        <v>604.68999999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16">
+        <v>76.320000000000007</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
+      </c>
+      <c r="J16">
+        <v>4508.25</v>
+      </c>
+      <c r="M16" t="s">
+        <v>55</v>
+      </c>
+      <c r="N16">
+        <v>566.57000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17">
+        <v>76.2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>56</v>
+      </c>
+      <c r="J17">
+        <v>6584.7</v>
+      </c>
+      <c r="M17" t="s">
+        <v>56</v>
+      </c>
+      <c r="N17">
+        <v>569.34</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18">
+        <v>82.43</v>
+      </c>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18">
+        <v>3067.3199999999997</v>
+      </c>
+      <c r="M18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18">
+        <v>602.41999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="5:14" x14ac:dyDescent="0.15">
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E40" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.15">
+      <c r="E41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4951,7 +7924,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated d/a/t charts with same-weight comparison
</commit_message>
<xml_diff>
--- a/CW1/results/results.xlsx
+++ b/CW1/results/results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4AE186-8856-994C-8796-E1C5F09BEE7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE30C756-F367-4F3B-8455-ABEF911780E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="62">
   <si>
     <t>lines map</t>
   </si>
@@ -215,6 +217,22 @@
     <t>A* Diagonal 10</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>Weight</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight 1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight 0.5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight 10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -224,7 +242,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -232,13 +250,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -246,7 +264,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -254,7 +272,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -318,7 +336,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -392,7 +410,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -734,7 +752,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1142320776"/>
@@ -794,7 +812,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1142325696"/>
@@ -836,7 +854,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -866,7 +884,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -880,7 +898,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -911,9 +929,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Total Distance on Factory Map</a:t>
             </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -942,7 +965,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -958,11 +981,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$F$12</c:f>
+              <c:f>Sheet2!$I$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>total distance</c:v>
+                  <c:v>A* Euclidean</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -979,36 +1002,27 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$E$13:$E$18</c:f>
+              <c:f>Sheet2!$J$27:$L$28</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>A* Euclidean</c:v>
+                  <c:v>Weight 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>A* Euclidean 0.5</c:v>
+                  <c:v>Weight 0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>A* Euclidean 10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>A* Diagonal</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>A* Diagonal 0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>A* Diagonal 10</c:v>
+                  <c:v>Weight 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$F$13:$F$18</c:f>
+              <c:f>Sheet2!$J$29:$L$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>76.69</c:v>
                 </c:pt>
@@ -1017,22 +1031,78 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>83.5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>76.320000000000007</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>76.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>82.43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4FDE-4CD6-8C45-C7A638379629}"/>
+              <c16:uniqueId val="{00000000-3CED-4047-AAC2-0167AFECBE8E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$I$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* Diagonal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$J$27:$L$28</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Weight 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Weight 0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weight 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$30:$L$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>76.320000000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.43</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3CED-4047-AAC2-0167AFECBE8E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1046,11 +1116,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="801989376"/>
-        <c:axId val="801993968"/>
+        <c:axId val="836462048"/>
+        <c:axId val="836468936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="801989376"/>
+        <c:axId val="836462048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,10 +1160,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="801993968"/>
+        <c:crossAx val="836468936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1101,7 +1171,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="801993968"/>
+        <c:axId val="836468936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1149,10 +1219,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="801989376"/>
+        <c:crossAx val="836462048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1164,6 +1234,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1190,7 +1291,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1204,7 +1305,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1235,16 +1336,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" altLang="zh-CN"/>
+              <a:rPr lang="en-GB" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Total Angle </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>on Factory Map</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB" altLang="zh-CN"/>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1273,7 +1378,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1289,11 +1394,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$J$12</c:f>
+              <c:f>Sheet2!$I$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>total Angle</c:v>
+                  <c:v>A* Euclidean</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1310,36 +1415,27 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$I$13:$I$18</c:f>
+              <c:f>Sheet2!$J$33:$L$34</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>A* Euclidean</c:v>
+                  <c:v>Weight 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>A* Euclidean 0.5</c:v>
+                  <c:v>Weight 0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>A* Euclidean 10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>A* Diagonal</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>A* Diagonal 0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>A* Diagonal 10</c:v>
+                  <c:v>Weight 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$J$13:$J$18</c:f>
+              <c:f>Sheet2!$J$35:$L$35</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>4732.5</c:v>
                 </c:pt>
@@ -1348,22 +1444,78 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4301.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4508.25</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6584.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3067.3199999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EC70-48D9-AE6B-926A05611346}"/>
+              <c16:uniqueId val="{00000000-8595-4D26-90D3-849BBF713B09}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$I$36</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* Diagonal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$J$33:$L$34</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Weight 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Weight 0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weight 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$36:$L$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4508.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6584.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3067.3199999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8595-4D26-90D3-849BBF713B09}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1377,11 +1529,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="807353728"/>
-        <c:axId val="807357336"/>
+        <c:axId val="841208216"/>
+        <c:axId val="841203296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="807353728"/>
+        <c:axId val="841208216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1421,10 +1573,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="807357336"/>
+        <c:crossAx val="841203296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1432,7 +1584,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="807357336"/>
+        <c:axId val="841203296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1480,10 +1632,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="807353728"/>
+        <c:crossAx val="841208216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1495,6 +1647,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1521,7 +1704,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1535,7 +1718,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1566,16 +1749,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" altLang="zh-CN"/>
+              <a:rPr lang="en-GB" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
               <a:t>Total Time </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>on Factory Map</a:t>
             </a:r>
-            <a:endParaRPr lang="en-GB" altLang="zh-CN"/>
+            <a:endParaRPr lang="zh-CN" altLang="zh-CN" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1604,7 +1791,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1620,11 +1807,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$N$12</c:f>
+              <c:f>Sheet2!$I$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>total time</c:v>
+                  <c:v>A* Euclidean</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1641,36 +1828,27 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet2!$M$13:$M$18</c:f>
+              <c:f>Sheet2!$J$38:$L$39</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>A* Euclidean</c:v>
+                  <c:v>Weight 1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>A* Euclidean 0.5</c:v>
+                  <c:v>Weight 0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>A* Euclidean 10</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>A* Diagonal</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>A* Diagonal 0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>A* Diagonal 10</c:v>
+                  <c:v>Weight 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$N$13:$N$18</c:f>
+              <c:f>Sheet2!$J$40:$L$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>563.32000000000005</c:v>
                 </c:pt>
@@ -1679,22 +1857,78 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>604.68999999999994</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>566.57000000000005</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>569.34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>602.41999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0A3E-4508-83CD-926A96AAD2BD}"/>
+              <c16:uniqueId val="{00000000-D2AE-491E-8878-1D88716C6D24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$I$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>A* Diagonal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$J$38:$L$39</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Weight 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Weight 0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Weight 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$41:$L$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>566.57000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>569.34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>602.41999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D2AE-491E-8878-1D88716C6D24}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1708,11 +1942,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="802013648"/>
-        <c:axId val="802016928"/>
+        <c:axId val="842900360"/>
+        <c:axId val="842900688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="802013648"/>
+        <c:axId val="842900360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,10 +1986,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="802016928"/>
+        <c:crossAx val="842900688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1763,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="802016928"/>
+        <c:axId val="842900688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1811,10 +2045,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="802013648"/>
+        <c:crossAx val="842900360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1826,6 +2060,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1852,7 +2117,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4075,23 +4340,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>918483</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>11338</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>376465</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>33109</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="7" name="Chart 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A77BDF6-25E5-42DD-90A5-511CBDAB1929}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E956D43F-DC2B-4A00-AE20-44439DFC4167}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4113,23 +4378,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>884464</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>113392</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>342446</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>135164</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="8" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4083E13C-5FE3-4631-95F0-11ECD7BAE8FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B31B7DE5-6F45-4183-B1FB-F5821B41DEA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4151,23 +4416,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>430892</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>79374</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>240392</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>101146</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEA3AB57-6D75-4C20-8001-41D7C81DC6AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72A66476-277B-4D8A-9070-B5D607513391}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4513,23 +4778,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="211" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="K57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T133" sqref="T133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="4" max="5" width="10.5" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.125" customWidth="1"/>
     <col min="10" max="10" width="10.5" customWidth="1"/>
-    <col min="11" max="11" width="25.1640625" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.125" customWidth="1"/>
+    <col min="13" max="13" width="13.625" customWidth="1"/>
     <col min="14" max="14" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -4567,12 +4832,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4613,7 +4878,7 @@
         <v>1330</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4654,7 +4919,7 @@
         <v>93.86</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -4695,7 +4960,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -4736,7 +5001,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -4777,12 +5042,12 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -4823,7 +5088,7 @@
         <v>1629</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -4864,7 +5129,7 @@
         <v>108.21</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -4905,7 +5170,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -4946,7 +5211,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -4987,12 +5252,12 @@
         <v>945</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -5033,7 +5298,7 @@
         <v>1675</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -5074,7 +5339,7 @@
         <v>110.01</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -5115,7 +5380,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -5156,7 +5421,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -5197,12 +5462,12 @@
         <v>720</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -5243,7 +5508,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -5284,7 +5549,7 @@
         <v>62.66</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -5325,7 +5590,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -5366,7 +5631,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -5407,7 +5672,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B31" t="s">
         <v>18</v>
       </c>
@@ -5445,12 +5710,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -5491,7 +5756,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -5532,7 +5797,7 @@
         <v>66.52</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -5573,7 +5838,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -5614,7 +5879,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -5655,12 +5920,12 @@
         <v>270</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>3</v>
       </c>
@@ -5701,7 +5966,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>1</v>
       </c>
@@ -5742,7 +6007,7 @@
         <v>115.1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -5783,7 +6048,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -5824,7 +6089,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -5865,7 +6130,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
         <v>11</v>
       </c>
@@ -5880,7 +6145,7 @@
       <c r="J47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
         <v>3</v>
       </c>
@@ -5921,7 +6186,7 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
         <v>1</v>
       </c>
@@ -5962,7 +6227,7 @@
         <v>116.2</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
         <v>2</v>
       </c>
@@ -6003,7 +6268,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
         <v>6</v>
       </c>
@@ -6044,7 +6309,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -6085,7 +6350,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -6093,7 +6358,7 @@
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -6101,7 +6366,7 @@
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
       <c r="B55" t="s">
         <v>18</v>
       </c>
@@ -6139,12 +6404,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
       <c r="E57" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
         <v>33</v>
       </c>
@@ -6152,7 +6417,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
         <v>23</v>
       </c>
@@ -6187,7 +6452,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>24</v>
       </c>
@@ -6223,7 +6488,7 @@
         <v>20.61</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A63" t="s">
         <v>25</v>
       </c>
@@ -6259,7 +6524,7 @@
         <v>1851.29</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -6295,7 +6560,7 @@
         <v>158.47</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
         <v>1</v>
       </c>
@@ -6304,15 +6569,15 @@
       <c r="K65" s="4"/>
       <c r="L65" s="4"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A66" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A67" s="1"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>31</v>
       </c>
@@ -6320,7 +6585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A69" t="s">
         <v>24</v>
       </c>
@@ -6356,7 +6621,7 @@
         <v>20.48</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A70" t="s">
         <v>25</v>
       </c>
@@ -6392,7 +6657,7 @@
         <v>1281.3499999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -6428,17 +6693,17 @@
         <v>151.43</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A75" t="s">
         <v>32</v>
       </c>
@@ -6446,7 +6711,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A76" t="s">
         <v>24</v>
       </c>
@@ -6482,7 +6747,7 @@
         <v>21.9</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>25</v>
       </c>
@@ -6518,7 +6783,7 @@
         <v>2868.05</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A78" t="s">
         <v>26</v>
       </c>
@@ -6554,7 +6819,7 @@
         <v>179.47</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A79" s="1" t="s">
         <v>1</v>
       </c>
@@ -6563,7 +6828,7 @@
       <c r="K79" s="4"/>
       <c r="L79" s="4"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
         <v>7</v>
       </c>
@@ -6572,7 +6837,7 @@
       <c r="K80" s="4"/>
       <c r="L80" s="4"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A82" t="s">
         <v>35</v>
       </c>
@@ -6581,7 +6846,7 @@
       <c r="J82" s="4"/>
       <c r="K82" s="4"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>24</v>
       </c>
@@ -6605,7 +6870,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A84" t="s">
         <v>25</v>
       </c>
@@ -6641,7 +6906,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A85" t="s">
         <v>26</v>
       </c>
@@ -6677,7 +6942,7 @@
         <v>20.49</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>1</v>
       </c>
@@ -6698,7 +6963,7 @@
       <c r="K86" s="4"/>
       <c r="L86" s="4"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
@@ -6719,7 +6984,7 @@
       <c r="K87" s="4"/>
       <c r="L87" s="4"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.15">
       <c r="H88" t="s">
         <v>25</v>
       </c>
@@ -6736,7 +7001,7 @@
         <v>1131.79</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A89" t="s">
         <v>36</v>
       </c>
@@ -6756,7 +7021,7 @@
         <v>152.51</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A90" t="s">
         <v>24</v>
       </c>
@@ -6777,7 +7042,7 @@
         <v>76.2</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A91" t="s">
         <v>25</v>
       </c>
@@ -6801,7 +7066,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A92" t="s">
         <v>26</v>
       </c>
@@ -6837,7 +7102,7 @@
         <v>20.48</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A93" s="1" t="s">
         <v>1</v>
       </c>
@@ -6858,7 +7123,7 @@
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
@@ -6879,7 +7144,7 @@
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.15">
       <c r="H95" t="s">
         <v>25</v>
       </c>
@@ -6896,7 +7161,7 @@
         <v>1300.8399999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A96" t="s">
         <v>37</v>
       </c>
@@ -6916,7 +7181,7 @@
         <v>153.76</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A97" t="s">
         <v>24</v>
       </c>
@@ -6937,7 +7202,7 @@
         <v>82.43</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A98" t="s">
         <v>25</v>
       </c>
@@ -6958,7 +7223,7 @@
         <v>3067.3199999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A99" t="s">
         <v>26</v>
       </c>
@@ -6982,7 +7247,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
         <v>1</v>
       </c>
@@ -7014,7 +7279,7 @@
         <v>24.82</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A101" s="1" t="s">
         <v>7</v>
       </c>
@@ -7046,7 +7311,7 @@
         <v>1249.6600000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.15">
       <c r="H102" t="s">
         <v>26</v>
       </c>
@@ -7063,7 +7328,7 @@
         <v>187.91</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B107" t="s">
         <v>12</v>
       </c>
@@ -7086,7 +7351,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.15">
       <c r="C108">
         <v>8.5</v>
       </c>
@@ -7109,7 +7374,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B109">
         <v>0</v>
       </c>
@@ -7153,7 +7418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B110">
         <v>0</v>
       </c>
@@ -7200,7 +7465,7 @@
         <v>4.7000000000000011</v>
       </c>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B111">
         <v>0</v>
       </c>
@@ -7247,7 +7512,7 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B112">
         <v>0</v>
       </c>
@@ -7294,7 +7559,7 @@
         <v>0.73428571428571432</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B113">
         <v>0</v>
       </c>
@@ -7317,7 +7582,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B114" s="1">
         <v>0</v>
       </c>
@@ -7340,7 +7605,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A115" s="3" t="s">
         <v>39</v>
       </c>
@@ -7376,7 +7641,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.15">
       <c r="L116" t="s">
         <v>12</v>
       </c>
@@ -7399,7 +7664,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.15">
       <c r="K117" t="s">
         <v>44</v>
       </c>
@@ -7429,7 +7694,7 @@
         <v>0.52139461172741697</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B118">
         <v>0.14000000000000001</v>
       </c>
@@ -7482,7 +7747,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B119">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -7533,7 +7798,7 @@
         <v>0.65477707006369434</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B120">
         <v>0</v>
       </c>
@@ -7556,7 +7821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B121">
         <v>0.01</v>
       </c>
@@ -7579,7 +7844,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B122">
         <v>0.27</v>
       </c>
@@ -7602,7 +7867,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B123" s="3">
         <v>0.27</v>
       </c>
@@ -7625,7 +7890,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A124" s="3" t="s">
         <v>40</v>
       </c>
@@ -7657,7 +7922,7 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B126">
         <v>1.1000000000000001</v>
       </c>
@@ -7680,7 +7945,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B127">
         <v>2.34</v>
       </c>
@@ -7703,7 +7968,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B128">
         <v>0.86</v>
       </c>
@@ -7726,7 +7991,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B129">
         <v>0.04</v>
       </c>
@@ -7749,7 +8014,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B130">
         <v>0.05</v>
       </c>
@@ -7772,7 +8037,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B131" s="3">
         <v>1.63</v>
       </c>
@@ -7795,7 +8060,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B132">
         <v>1.83</v>
       </c>
@@ -7818,7 +8083,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A133" t="s">
         <v>41</v>
       </c>
@@ -7861,19 +8126,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="E11:N41"/>
+  <dimension ref="D11:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12:N18"/>
+    <sheetView topLeftCell="C12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="5" max="5" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.125" customWidth="1"/>
+    <col min="9" max="9" width="21.875" customWidth="1"/>
+    <col min="13" max="13" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="11" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
+    <row r="11" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D11" t="s">
         <v>48</v>
       </c>
       <c r="I11" t="s">
@@ -7883,9 +8150,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
         <v>24</v>
@@ -7903,9 +8173,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E13" t="s">
+    <row r="13" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D13" t="s">
         <v>52</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
       </c>
       <c r="F13">
         <v>76.69</v>
@@ -7923,9 +8196,12 @@
         <v>563.32000000000005</v>
       </c>
     </row>
-    <row r="14" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E14" t="s">
-        <v>53</v>
+    <row r="14" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>0.5</v>
       </c>
       <c r="F14">
         <v>75.959999999999994</v>
@@ -7943,9 +8219,12 @@
         <v>557.67999999999995</v>
       </c>
     </row>
-    <row r="15" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E15" t="s">
-        <v>54</v>
+    <row r="15" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
       </c>
       <c r="F15">
         <v>83.5</v>
@@ -7963,9 +8242,12 @@
         <v>604.68999999999994</v>
       </c>
     </row>
-    <row r="16" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E16" t="s">
+    <row r="16" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D16" t="s">
         <v>55</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
       <c r="F16">
         <v>76.320000000000007</v>
@@ -7983,9 +8265,12 @@
         <v>566.57000000000005</v>
       </c>
     </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E17" t="s">
-        <v>56</v>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17">
+        <v>0.5</v>
       </c>
       <c r="F17">
         <v>76.2</v>
@@ -8003,9 +8288,12 @@
         <v>569.34</v>
       </c>
     </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.2">
-      <c r="E18" t="s">
-        <v>57</v>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
       </c>
       <c r="F18">
         <v>82.43</v>
@@ -8023,49 +8311,165 @@
         <v>602.41999999999996</v>
       </c>
     </row>
-    <row r="29" spans="5:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="I27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.15">
+      <c r="J28" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.15">
       <c r="E29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29">
+        <v>76.69</v>
+      </c>
+      <c r="K29">
+        <v>75.959999999999994</v>
+      </c>
+      <c r="L29">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.15">
       <c r="E30" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30">
+        <v>76.320000000000007</v>
+      </c>
+      <c r="K30">
+        <v>76.2</v>
+      </c>
+      <c r="L30">
+        <v>82.43</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.15">
       <c r="E31" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="I33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E34" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>59</v>
+      </c>
+      <c r="K34" t="s">
+        <v>60</v>
+      </c>
+      <c r="L34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E35" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>52</v>
+      </c>
+      <c r="J35">
+        <v>4732.5</v>
+      </c>
+      <c r="K35">
+        <v>4215.7199999999993</v>
+      </c>
+      <c r="L35">
+        <v>4301.2</v>
+      </c>
+    </row>
+    <row r="36" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E36" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>55</v>
+      </c>
+      <c r="J36">
+        <v>4508.25</v>
+      </c>
+      <c r="K36">
+        <v>6584.7</v>
+      </c>
+      <c r="L36">
+        <v>3067.3199999999997</v>
+      </c>
+    </row>
+    <row r="38" spans="5:12" x14ac:dyDescent="0.15">
+      <c r="I38" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E39" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>59</v>
+      </c>
+      <c r="K39" t="s">
+        <v>60</v>
+      </c>
+      <c r="L39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E40" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40">
+        <v>563.32000000000005</v>
+      </c>
+      <c r="K40">
+        <v>557.67999999999995</v>
+      </c>
+      <c r="L40">
+        <v>604.68999999999994</v>
+      </c>
+    </row>
+    <row r="41" spans="5:12" x14ac:dyDescent="0.15">
       <c r="E41" t="s">
         <v>26</v>
+      </c>
+      <c r="I41" t="s">
+        <v>55</v>
+      </c>
+      <c r="J41">
+        <v>566.57000000000005</v>
+      </c>
+      <c r="K41">
+        <v>569.34</v>
+      </c>
+      <c r="L41">
+        <v>602.41999999999996</v>
       </c>
     </row>
   </sheetData>
@@ -8081,7 +8485,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>